<commit_message>
Buổi 11: hệ thống lại router + layout
</commit_message>
<xml_diff>
--- a/diem_danh_giay_07_03_23_03_27_07.xlsx
+++ b/diem_danh_giay_07_03_23_03_27_07.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="16400"/>
+    <workbookView windowHeight="18800"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -426,10 +426,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -474,7 +474,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -496,18 +496,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -520,22 +520,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -557,7 +542,22 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -566,22 +566,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -594,17 +587,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -625,13 +625,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -643,7 +703,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,7 +715,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -667,37 +775,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -709,97 +793,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,11 +837,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -861,17 +893,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -890,156 +925,121 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1048,22 +1048,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1488,8 +1488,8 @@
   <sheetPr/>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="215" zoomScaleNormal="215" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2011,7 +2011,9 @@
       <c r="E15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>4</v>
+      </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2125,7 +2127,9 @@
       <c r="E18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="1">
+        <v>4</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2163,7 +2167,9 @@
       <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="1">
+        <v>4</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -2353,7 +2359,9 @@
       <c r="E24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1">
+        <v>4</v>
+      </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -2391,7 +2399,9 @@
       <c r="E25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="1">
+        <v>4</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2809,7 +2819,9 @@
       <c r="E36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="1">
+        <v>4</v>
+      </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -2885,7 +2897,9 @@
       <c r="E38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="1">
+        <v>4</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>

</xml_diff>